<commit_message>
adding site info to manu
</commit_message>
<xml_diff>
--- a/data/zombie3.xlsx
+++ b/data/zombie3.xlsx
@@ -406,187 +406,187 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>152</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>222</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>264</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>297</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>343</v>
+        <v>442</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>442</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>455</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>500</v>
+        <v>677</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>677</v>
+        <v>689</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>689</v>
+        <v>695</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>695</v>
+        <v>731</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>731</v>
+        <v>753</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>753</v>
+        <v>761</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>761</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1245</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1392</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1447</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1529</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>119</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>137</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>156</v>
+        <v>679</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>189</v>
+        <v>682</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>449</v>
+        <v>704</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>679</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>682</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>704</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>1473</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>1475</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>74</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed outliers, updated graphs
</commit_message>
<xml_diff>
--- a/data/zombie3.xlsx
+++ b/data/zombie3.xlsx
@@ -421,147 +421,147 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>343</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>442</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>455</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>500</v>
+        <v>677</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>677</v>
+        <v>689</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>689</v>
+        <v>695</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>695</v>
+        <v>731</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>731</v>
+        <v>753</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>753</v>
+        <v>761</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>761</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1245</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1392</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1447</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1529</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>119</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>189</v>
+        <v>449</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>449</v>
+        <v>679</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>682</v>
+        <v>704</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>704</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>1473</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>1475</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42">

</xml_diff>